<commit_message>
them tim kim theo de
</commit_message>
<xml_diff>
--- a/ExamServer/ExamPapers/exam_DT001.xlsx
+++ b/ExamServer/ExamPapers/exam_DT001.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\School Projects\2025_K18_SD1802_PRO231\Assignment\PRO231_ExamApp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dell\source\repos\gachienmam\PRO231_ExamApp\ExamServer\ExamPapers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A59C5982-60BF-49E1-BEA5-B6A58F3C94EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{463230CF-1A84-4048-91CC-8904F8CB6086}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21705" yWindow="5550" windowWidth="14145" windowHeight="9045" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Thong Tin" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="26">
   <si>
     <t>C</t>
   </si>
@@ -81,6 +81,30 @@
   </si>
   <si>
     <t>QuestionAnswers</t>
+  </si>
+  <si>
+    <t>1+1=</t>
+  </si>
+  <si>
+    <t>2+2=</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>3+3=</t>
+  </si>
+  <si>
+    <t>4+4=</t>
+  </si>
+  <si>
+    <t>5+5=</t>
+  </si>
+  <si>
+    <t>6+6=</t>
+  </si>
+  <si>
+    <t>7+7=</t>
   </si>
 </sst>
 </file>
@@ -88,27 +112,27 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="1">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1" tint="0.24994659260841701"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -145,7 +169,7 @@
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
@@ -187,26 +211,6 @@
   <dxfs count="30">
     <dxf>
       <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -246,68 +250,6 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11"/>
-        <color rgb="FF44546A"/>
-        <name val="Franklin Gothic Medium"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF000000"/>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <name val="Franklin Gothic Medium"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF000000"/>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="5" tint="-0.749992370372631"/>
-        <name val="Franklin Gothic Medium"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
         <name val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -361,90 +303,6 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11"/>
-        <color theme="3"/>
-        <name val="Franklin Gothic Medium"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <name val="Franklin Gothic Medium"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="5" tint="-0.749992370372631"/>
-        <name val="Franklin Gothic Medium"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="5" tint="-0.749992370372631"/>
-        <name val="Franklin Gothic Medium"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
         <name val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -724,6 +582,68 @@
     </dxf>
     <dxf>
       <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="3"/>
+        <name val="Franklin Gothic Medium"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Franklin Gothic Medium"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="5" tint="-0.749992370372631"/>
+        <name val="Franklin Gothic Medium"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -777,6 +697,68 @@
     </dxf>
     <dxf>
       <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF44546A"/>
+        <name val="Franklin Gothic Medium"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF000000"/>
+          <bgColor rgb="FFF2F2F2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Franklin Gothic Medium"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF000000"/>
+          <bgColor rgb="FFF2F2F2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="5" tint="-0.749992370372631"/>
+        <name val="Franklin Gothic Medium"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -816,6 +798,26 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
         <color theme="3"/>
         <name val="Franklin Gothic Medium"/>
         <family val="2"/>
@@ -847,6 +849,28 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="5" tint="-0.749992370372631"/>
+        <name val="Franklin Gothic Medium"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -935,10 +959,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8F7A7EF5-B089-4716-BD92-FB40E5E39317}" name="MultipleChoiceData3" displayName="MultipleChoiceData3" ref="A1:A2" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8" totalsRowDxfId="7" headerRowCellStyle="Header Row">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8F7A7EF5-B089-4716-BD92-FB40E5E39317}" name="MultipleChoiceData3" displayName="MultipleChoiceData3" ref="A1:A2" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25" totalsRowDxfId="24" headerRowCellStyle="Header Row">
   <autoFilter ref="A1:A2" xr:uid="{8F7A7EF5-B089-4716-BD92-FB40E5E39317}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{A09D6441-B594-4101-BF76-D433E4EB42EE}" name="ThoiGianLamBai" dataDxfId="5" totalsRowDxfId="6" dataCellStyle="Date"/>
+    <tableColumn id="1" xr3:uid="{A09D6441-B594-4101-BF76-D433E4EB42EE}" name="ThoiGianLamBai" dataDxfId="23" totalsRowDxfId="22" dataCellStyle="Date"/>
   </tableColumns>
   <tableStyleInfo name="Business Table" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
   <extLst>
@@ -950,10 +974,10 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{2BA0DD7C-6178-4B89-B8BA-4FF70FFF6D2F}" name="MultipleChoiceData34" displayName="MultipleChoiceData34" ref="A1:A2" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3" totalsRowDxfId="2" headerRowCellStyle="Header Row">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{2BA0DD7C-6178-4B89-B8BA-4FF70FFF6D2F}" name="MultipleChoiceData34" displayName="MultipleChoiceData34" ref="A1:A2" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20" totalsRowDxfId="19" headerRowCellStyle="Header Row">
   <autoFilter ref="A1:A2" xr:uid="{8F7A7EF5-B089-4716-BD92-FB40E5E39317}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{6CCBC175-B30E-4A0B-8A0A-9F5908478785}" name="XaoTronCauHoi" dataDxfId="0" totalsRowDxfId="1" dataCellStyle="Date"/>
+    <tableColumn id="1" xr3:uid="{6CCBC175-B30E-4A0B-8A0A-9F5908478785}" name="XaoTronCauHoi" dataDxfId="18" totalsRowDxfId="17" dataCellStyle="Date"/>
   </tableColumns>
   <tableStyleInfo name="Business Table" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
   <extLst>
@@ -965,16 +989,16 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00ACF1BA-5F02-4145-A0BB-6DAC54008E3C}" name="MultipleChoiceData" displayName="MultipleChoiceData" ref="A1:G4" totalsRowShown="0" headerRowDxfId="10" dataDxfId="26" totalsRowDxfId="25" headerRowCellStyle="Header Row">
-  <autoFilter ref="A1:G4" xr:uid="{00ACF1BA-5F02-4145-A0BB-6DAC54008E3C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00ACF1BA-5F02-4145-A0BB-6DAC54008E3C}" name="MultipleChoiceData" displayName="MultipleChoiceData" ref="A1:G11" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15" totalsRowDxfId="14" headerRowCellStyle="Header Row">
+  <autoFilter ref="A1:G11" xr:uid="{00ACF1BA-5F02-4145-A0BB-6DAC54008E3C}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{847969CD-F3EA-46D8-9085-38E4E10A78A0}" name="QuestionID" dataDxfId="23" totalsRowDxfId="24" dataCellStyle="Date"/>
-    <tableColumn id="2" xr3:uid="{1FBA4876-8B22-485A-ABEE-ECEDC1B283CA}" name="QuestionText" dataDxfId="21" totalsRowDxfId="22" dataCellStyle="Table Text"/>
-    <tableColumn id="3" xr3:uid="{77DFD0B2-B276-42E9-A09C-DCD3365A0235}" name="QuestionAnswerTextA" dataDxfId="19" totalsRowDxfId="20" dataCellStyle="Table Text"/>
-    <tableColumn id="4" xr3:uid="{06A7C2AF-5FBA-4570-A0A7-BC9A956B596D}" name="QuestionAnswerTextB" dataDxfId="17" totalsRowDxfId="18" dataCellStyle="Table Text"/>
-    <tableColumn id="5" xr3:uid="{8227EC02-757E-4F50-A180-88810D6D0779}" name="QuestionAnswerTextC" dataDxfId="15" totalsRowDxfId="16" dataCellStyle="Currency"/>
-    <tableColumn id="6" xr3:uid="{F004C90B-0884-4D5D-B41A-BB17E69AC7D4}" name="QuestionAnswerTextD" dataDxfId="13" totalsRowDxfId="14" dataCellStyle="Currency"/>
-    <tableColumn id="7" xr3:uid="{A2F259B7-5F21-4EA5-B2E3-FD4A4B51A497}" name="QuestionAnswers" dataDxfId="11" totalsRowDxfId="12" dataCellStyle="Currency"/>
+    <tableColumn id="1" xr3:uid="{847969CD-F3EA-46D8-9085-38E4E10A78A0}" name="QuestionID" dataDxfId="13" totalsRowDxfId="12" dataCellStyle="Date"/>
+    <tableColumn id="2" xr3:uid="{1FBA4876-8B22-485A-ABEE-ECEDC1B283CA}" name="QuestionText" dataDxfId="11" totalsRowDxfId="10" dataCellStyle="Table Text"/>
+    <tableColumn id="3" xr3:uid="{77DFD0B2-B276-42E9-A09C-DCD3365A0235}" name="QuestionAnswerTextA" dataDxfId="9" totalsRowDxfId="8" dataCellStyle="Table Text"/>
+    <tableColumn id="4" xr3:uid="{06A7C2AF-5FBA-4570-A0A7-BC9A956B596D}" name="QuestionAnswerTextB" dataDxfId="7" totalsRowDxfId="6" dataCellStyle="Table Text"/>
+    <tableColumn id="5" xr3:uid="{8227EC02-757E-4F50-A180-88810D6D0779}" name="QuestionAnswerTextC" dataDxfId="5" totalsRowDxfId="4" dataCellStyle="Currency"/>
+    <tableColumn id="6" xr3:uid="{F004C90B-0884-4D5D-B41A-BB17E69AC7D4}" name="QuestionAnswerTextD" dataDxfId="3" totalsRowDxfId="2" dataCellStyle="Currency"/>
+    <tableColumn id="7" xr3:uid="{A2F259B7-5F21-4EA5-B2E3-FD4A4B51A497}" name="QuestionAnswers" dataDxfId="1" totalsRowDxfId="0" dataCellStyle="Currency"/>
   </tableColumns>
   <tableStyleInfo name="Business Table" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
   <extLst>
@@ -1254,17 +1278,17 @@
       <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.59765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="7.3984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.3984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.8984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" ht="16.2" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>8</v>
       </c>
@@ -1293,17 +1317,17 @@
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.59765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="7.3984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.3984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.8984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" ht="16.2" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>9</v>
       </c>
@@ -1326,23 +1350,23 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{517730C4-EE94-4B85-9F73-4AA1607F57C0}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="30.09765625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="30" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.09765625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="16.2" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>11</v>
       </c>
@@ -1365,7 +1389,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1388,7 +1412,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1432,6 +1456,167 @@
       </c>
       <c r="G4" s="4" t="s">
         <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="2">
+        <v>1</v>
+      </c>
+      <c r="D5" s="2">
+        <v>2</v>
+      </c>
+      <c r="E5" s="2">
+        <v>3</v>
+      </c>
+      <c r="F5" s="2">
+        <v>4</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="2">
+        <v>1</v>
+      </c>
+      <c r="D6" s="2">
+        <v>2</v>
+      </c>
+      <c r="E6" s="2">
+        <v>3</v>
+      </c>
+      <c r="F6" s="2">
+        <v>4</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="2">
+        <v>3</v>
+      </c>
+      <c r="D7" s="2">
+        <v>6</v>
+      </c>
+      <c r="E7" s="2">
+        <v>9</v>
+      </c>
+      <c r="F7" s="2">
+        <v>12</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="2">
+        <v>4</v>
+      </c>
+      <c r="D8" s="2">
+        <v>8</v>
+      </c>
+      <c r="E8" s="2">
+        <v>12</v>
+      </c>
+      <c r="F8" s="2">
+        <v>16</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="2">
+        <v>5</v>
+      </c>
+      <c r="D9" s="2">
+        <v>10</v>
+      </c>
+      <c r="E9" s="2">
+        <v>15</v>
+      </c>
+      <c r="F9" s="2">
+        <v>25</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="2">
+        <v>6</v>
+      </c>
+      <c r="D10" s="2">
+        <v>12</v>
+      </c>
+      <c r="E10" s="2">
+        <v>15</v>
+      </c>
+      <c r="F10" s="2">
+        <v>36</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="2">
+        <v>7</v>
+      </c>
+      <c r="D11" s="2">
+        <v>3</v>
+      </c>
+      <c r="E11" s="2">
+        <v>7</v>
+      </c>
+      <c r="F11" s="2">
+        <v>49</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implement putting images in exam and for each question, and other modifications to ManagementApp forms
</commit_message>
<xml_diff>
--- a/ExamServer/ExamPapers/exam_DT001.xlsx
+++ b/ExamServer/ExamPapers/exam_DT001.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dell\source\repos\gachienmam\PRO231_ExamApp\ExamServer\ExamPapers\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\School Projects\2025_K18_SD1802_PRO231\Assignment\PRO231_ExamApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{463230CF-1A84-4048-91CC-8904F8CB6086}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC81BF4B-B0A3-41B8-B0F0-247B9A306408}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16155" yWindow="3150" windowWidth="14145" windowHeight="9045" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Thong Tin" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="30">
   <si>
     <t>C</t>
   </si>
@@ -105,6 +105,18 @@
   </si>
   <si>
     <t>7+7=</t>
+  </si>
+  <si>
+    <t>QuestionImageLink</t>
+  </si>
+  <si>
+    <t>LinkAnhDeThi</t>
+  </si>
+  <si>
+    <t>https://media.discordapp.net/attachments/1356348075026677881/1356348101706911886/5916d9d9-4216-45a6-b971-0a234af38851.jpeg?ex=67ec3d1b&amp;is=67eaeb9b&amp;hm=7985e466675433d22f3877cac0fa41a1ef2752ad4c467ed3783001897de19c22&amp;=</t>
+  </si>
+  <si>
+    <t>https://media.discordapp.net/attachments/1356348075026677881/1356358814466838598/image.png?ex=67ec4715&amp;is=67eaf595&amp;hm=61bd7348ed87a8f0781410936df07f2e84bafd56aa112485416bb6fa9751021c&amp;=</t>
   </si>
 </sst>
 </file>
@@ -112,27 +124,27 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1" tint="0.24994659260841701"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -142,6 +154,20 @@
       <color theme="5" tint="-0.749992370372631"/>
       <name val="Franklin Gothic Medium"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1" tint="0.24994659260841701"/>
+      <name val="Franklin Gothic Medium"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -167,9 +193,9 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
@@ -179,8 +205,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -200,15 +227,75 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="44" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="2" borderId="0" xfId="5" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="6">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Date" xfId="3" xr:uid="{384076B8-EB15-4AA8-9AB8-14A35816E9B7}"/>
     <cellStyle name="Header Row" xfId="2" xr:uid="{5AD8A4AF-BF9F-4597-ACB1-4EF491A52F97}"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Table Text" xfId="4" xr:uid="{888AE7D8-C4DF-4345-B361-7FC4356C86C3}"/>
   </cellStyles>
-  <dxfs count="30">
+  <dxfs count="34">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="3"/>
+        <name val="Franklin Gothic Medium"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="medium">
+          <color theme="4" tint="-0.749992370372631"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Franklin Gothic Medium"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -749,6 +836,48 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="3"/>
+        <name val="Franklin Gothic Medium"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="medium">
+          <color theme="4" tint="-0.749992370372631"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -942,9 +1071,9 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Business Table" pivot="0" count="3" xr9:uid="{AC661F50-C690-4DA3-A207-6D7072D363DF}">
-      <tableStyleElement type="wholeTable" dxfId="29"/>
-      <tableStyleElement type="headerRow" dxfId="28"/>
-      <tableStyleElement type="totalRow" dxfId="27"/>
+      <tableStyleElement type="wholeTable" dxfId="33"/>
+      <tableStyleElement type="headerRow" dxfId="32"/>
+      <tableStyleElement type="totalRow" dxfId="31"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -959,10 +1088,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8F7A7EF5-B089-4716-BD92-FB40E5E39317}" name="MultipleChoiceData3" displayName="MultipleChoiceData3" ref="A1:A2" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25" totalsRowDxfId="24" headerRowCellStyle="Header Row">
-  <autoFilter ref="A1:A2" xr:uid="{8F7A7EF5-B089-4716-BD92-FB40E5E39317}"/>
-  <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{A09D6441-B594-4101-BF76-D433E4EB42EE}" name="ThoiGianLamBai" dataDxfId="23" totalsRowDxfId="22" dataCellStyle="Date"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8F7A7EF5-B089-4716-BD92-FB40E5E39317}" name="MultipleChoiceData3" displayName="MultipleChoiceData3" ref="A1:B2" totalsRowShown="0" headerRowDxfId="30" dataDxfId="29" totalsRowDxfId="28" headerRowCellStyle="Header Row">
+  <autoFilter ref="A1:B2" xr:uid="{8F7A7EF5-B089-4716-BD92-FB40E5E39317}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{A09D6441-B594-4101-BF76-D433E4EB42EE}" name="ThoiGianLamBai" dataDxfId="27" totalsRowDxfId="26" dataCellStyle="Date"/>
+    <tableColumn id="2" xr3:uid="{9EC7DAAC-F681-4CA0-998D-93C2CBC65297}" name="LinkAnhDeThi" dataDxfId="25" totalsRowDxfId="24" dataCellStyle="Hyperlink"/>
   </tableColumns>
   <tableStyleInfo name="Business Table" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
   <extLst>
@@ -974,10 +1104,10 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{2BA0DD7C-6178-4B89-B8BA-4FF70FFF6D2F}" name="MultipleChoiceData34" displayName="MultipleChoiceData34" ref="A1:A2" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20" totalsRowDxfId="19" headerRowCellStyle="Header Row">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{2BA0DD7C-6178-4B89-B8BA-4FF70FFF6D2F}" name="MultipleChoiceData34" displayName="MultipleChoiceData34" ref="A1:A2" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22" totalsRowDxfId="21" headerRowCellStyle="Header Row">
   <autoFilter ref="A1:A2" xr:uid="{8F7A7EF5-B089-4716-BD92-FB40E5E39317}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{6CCBC175-B30E-4A0B-8A0A-9F5908478785}" name="XaoTronCauHoi" dataDxfId="18" totalsRowDxfId="17" dataCellStyle="Date"/>
+    <tableColumn id="1" xr3:uid="{6CCBC175-B30E-4A0B-8A0A-9F5908478785}" name="XaoTronCauHoi" dataDxfId="20" totalsRowDxfId="19" dataCellStyle="Date"/>
   </tableColumns>
   <tableStyleInfo name="Business Table" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
   <extLst>
@@ -989,16 +1119,17 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00ACF1BA-5F02-4145-A0BB-6DAC54008E3C}" name="MultipleChoiceData" displayName="MultipleChoiceData" ref="A1:G11" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15" totalsRowDxfId="14" headerRowCellStyle="Header Row">
-  <autoFilter ref="A1:G11" xr:uid="{00ACF1BA-5F02-4145-A0BB-6DAC54008E3C}"/>
-  <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{847969CD-F3EA-46D8-9085-38E4E10A78A0}" name="QuestionID" dataDxfId="13" totalsRowDxfId="12" dataCellStyle="Date"/>
-    <tableColumn id="2" xr3:uid="{1FBA4876-8B22-485A-ABEE-ECEDC1B283CA}" name="QuestionText" dataDxfId="11" totalsRowDxfId="10" dataCellStyle="Table Text"/>
-    <tableColumn id="3" xr3:uid="{77DFD0B2-B276-42E9-A09C-DCD3365A0235}" name="QuestionAnswerTextA" dataDxfId="9" totalsRowDxfId="8" dataCellStyle="Table Text"/>
-    <tableColumn id="4" xr3:uid="{06A7C2AF-5FBA-4570-A0A7-BC9A956B596D}" name="QuestionAnswerTextB" dataDxfId="7" totalsRowDxfId="6" dataCellStyle="Table Text"/>
-    <tableColumn id="5" xr3:uid="{8227EC02-757E-4F50-A180-88810D6D0779}" name="QuestionAnswerTextC" dataDxfId="5" totalsRowDxfId="4" dataCellStyle="Currency"/>
-    <tableColumn id="6" xr3:uid="{F004C90B-0884-4D5D-B41A-BB17E69AC7D4}" name="QuestionAnswerTextD" dataDxfId="3" totalsRowDxfId="2" dataCellStyle="Currency"/>
-    <tableColumn id="7" xr3:uid="{A2F259B7-5F21-4EA5-B2E3-FD4A4B51A497}" name="QuestionAnswers" dataDxfId="1" totalsRowDxfId="0" dataCellStyle="Currency"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00ACF1BA-5F02-4145-A0BB-6DAC54008E3C}" name="MultipleChoiceData" displayName="MultipleChoiceData" ref="A1:H11" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17" totalsRowDxfId="16" headerRowCellStyle="Header Row">
+  <autoFilter ref="A1:H11" xr:uid="{00ACF1BA-5F02-4145-A0BB-6DAC54008E3C}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{847969CD-F3EA-46D8-9085-38E4E10A78A0}" name="QuestionID" dataDxfId="15" totalsRowDxfId="14" dataCellStyle="Date"/>
+    <tableColumn id="2" xr3:uid="{1FBA4876-8B22-485A-ABEE-ECEDC1B283CA}" name="QuestionText" dataDxfId="13" totalsRowDxfId="12" dataCellStyle="Table Text"/>
+    <tableColumn id="3" xr3:uid="{77DFD0B2-B276-42E9-A09C-DCD3365A0235}" name="QuestionAnswerTextA" dataDxfId="11" totalsRowDxfId="10" dataCellStyle="Table Text"/>
+    <tableColumn id="4" xr3:uid="{06A7C2AF-5FBA-4570-A0A7-BC9A956B596D}" name="QuestionAnswerTextB" dataDxfId="9" totalsRowDxfId="8" dataCellStyle="Table Text"/>
+    <tableColumn id="5" xr3:uid="{8227EC02-757E-4F50-A180-88810D6D0779}" name="QuestionAnswerTextC" dataDxfId="7" totalsRowDxfId="6" dataCellStyle="Currency"/>
+    <tableColumn id="6" xr3:uid="{F004C90B-0884-4D5D-B41A-BB17E69AC7D4}" name="QuestionAnswerTextD" dataDxfId="5" totalsRowDxfId="4" dataCellStyle="Currency"/>
+    <tableColumn id="7" xr3:uid="{A2F259B7-5F21-4EA5-B2E3-FD4A4B51A497}" name="QuestionAnswers" dataDxfId="3" totalsRowDxfId="2" dataCellStyle="Currency"/>
+    <tableColumn id="8" xr3:uid="{B9F616E2-9758-428E-AD07-14CFDE65EEF3}" name="QuestionImageLink" dataDxfId="1" totalsRowDxfId="0" dataCellStyle="Currency"/>
   </tableColumns>
   <tableStyleInfo name="Business Table" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
   <extLst>
@@ -1272,39 +1403,48 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.59765625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="7.3984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.3984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.8984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>8</v>
       </c>
+      <c r="B1" s="6" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>3600</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Date in this column under this heading" sqref="A1" xr:uid="{FD054FFF-883E-4599-9086-0768D060239E}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Date in this column under this heading" sqref="A1:B1" xr:uid="{FD054FFF-883E-4599-9086-0768D060239E}"/>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{DC29A595-1C43-474A-8532-4CF28CF18CBB}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -1317,17 +1457,17 @@
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.59765625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="7.3984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.3984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.8984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>9</v>
       </c>
@@ -1350,23 +1490,23 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{517730C4-EE94-4B85-9F73-4AA1607F57C0}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="30.09765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="30.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="30" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30.09765625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>11</v>
       </c>
@@ -1388,8 +1528,11 @@
       <c r="G1" s="6" t="s">
         <v>17</v>
       </c>
+      <c r="H1" s="6" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1411,8 +1554,11 @@
       <c r="G2" s="4" t="s">
         <v>7</v>
       </c>
+      <c r="H2" s="8" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1434,8 +1580,9 @@
       <c r="G3" s="4" t="s">
         <v>0</v>
       </c>
+      <c r="H3" s="7"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1457,8 +1604,9 @@
       <c r="G4" s="4" t="s">
         <v>1</v>
       </c>
+      <c r="H4" s="7"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1480,8 +1628,9 @@
       <c r="G5" s="4" t="s">
         <v>20</v>
       </c>
+      <c r="H5" s="7"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1503,8 +1652,9 @@
       <c r="G6" s="4" t="s">
         <v>1</v>
       </c>
+      <c r="H6" s="7"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1526,8 +1676,9 @@
       <c r="G7" s="4" t="s">
         <v>0</v>
       </c>
+      <c r="H7" s="7"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1549,8 +1700,9 @@
       <c r="G8" s="4" t="s">
         <v>20</v>
       </c>
+      <c r="H8" s="7"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1572,8 +1724,9 @@
       <c r="G9" s="4" t="s">
         <v>1</v>
       </c>
+      <c r="H9" s="7"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1595,8 +1748,9 @@
       <c r="G10" s="4" t="s">
         <v>0</v>
       </c>
+      <c r="H10" s="7"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1618,17 +1772,21 @@
       <c r="G11" s="4" t="s">
         <v>20</v>
       </c>
+      <c r="H11" s="7"/>
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Meal expenses in this column under this heading" sqref="G1" xr:uid="{70FDA402-9FB7-4C8A-B472-E9B5E0CBF1AA}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Meal expenses in this column under this heading" sqref="G1:H1" xr:uid="{70FDA402-9FB7-4C8A-B472-E9B5E0CBF1AA}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Description in this column under this heading" sqref="C1:F1" xr:uid="{FA7C5454-0B37-4A9B-971C-50A26A953225}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Account in this column under this heading" sqref="B1" xr:uid="{EBD3B7E9-5EF6-45B0-B86C-BA09256906A8}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Date in this column under this heading" sqref="A1" xr:uid="{488BF94A-1339-4E27-A840-00984148C6D5}"/>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="H2" r:id="rId1" xr:uid="{2CD79C5E-CEFB-422F-AAED-CBF40F2D0094}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>